<commit_message>
add preliminary text generation script
</commit_message>
<xml_diff>
--- a/projectPlanning/datasetsNotes.xlsx
+++ b/projectPlanning/datasetsNotes.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/projectPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2B10073-A359-6245-8F07-FB0B2CBCA12E}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE922010-6B76-B64B-B244-9AE4DAF3FFDB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datasets" sheetId="1" r:id="rId1"/>
+    <sheet name="AIPrompts" sheetId="2" r:id="rId2"/>
+    <sheet name="APIs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -180,13 +182,269 @@
   </si>
   <si>
     <t xml:space="preserve">STARTING WITH THIS DATASET. </t>
+  </si>
+  <si>
+    <t>essay_set</t>
+  </si>
+  <si>
+    <t>type_of_essay</t>
+  </si>
+  <si>
+    <t>Human Prompt</t>
+  </si>
+  <si>
+    <t>AI Prompt 1</t>
+  </si>
+  <si>
+    <t>grade_level</t>
+  </si>
+  <si>
+    <t>training_set_size</t>
+  </si>
+  <si>
+    <t>valid_set_size</t>
+  </si>
+  <si>
+    <t>test_set_size</t>
+  </si>
+  <si>
+    <t>min_domain1_score</t>
+  </si>
+  <si>
+    <t>max_domain1_score</t>
+  </si>
+  <si>
+    <t>min_domain2_score</t>
+  </si>
+  <si>
+    <t>max_domain2_score</t>
+  </si>
+  <si>
+    <t>has_domain1rater1</t>
+  </si>
+  <si>
+    <t>has_domain1rater2</t>
+  </si>
+  <si>
+    <t>has_domain1rater3</t>
+  </si>
+  <si>
+    <t>has_domain1_score</t>
+  </si>
+  <si>
+    <t>has_domain2rater1</t>
+  </si>
+  <si>
+    <t>has_domain2rater2</t>
+  </si>
+  <si>
+    <t>has_domain2_score</t>
+  </si>
+  <si>
+    <t>persuasive / narrative  / expository</t>
+  </si>
+  <si>
+    <t>More and more people use computers, but not everyone agrees that this benefits society. Those who support advances in technology believe that computers have a positive effect on people. They teach hand-eye coordination, give people the ability to learn about faraway places and people, and even allow people to talk online with other people. Others have different ideas. Some experts are concerned that people are spending too much time on their computers and less time exercising, enjoying nature, and interacting with family and friends. 
+Write a letter to your local newspaper in which you state your opinion on the effects computers have on people. Persuade the readers to agree with you.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response on the effects computers have on people. Persuade the readers to agree with your position.</t>
+  </si>
+  <si>
+    <t>Censorship in the Libraries
+"All of us can think of a book that we hope none of our children or any other children have taken off the shelf. But if I have the right to remove that book from the shelf -- that work I abhor -- then you also have exactly the same right and so does everyone else. And then we have no books left on the shelf for any of us." --Katherine Paterson, Author
+Write a persuasive essay to a newspaper reflecting your views on censorship in libraries. Do you believe that certain materials, such as books, music, movies, magazines, etc., should be removed from the shelves if they are found offensive? Support your position with convincing arguments from your own experience, observations, and/or reading.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response to the following prompt: Write a persuasive essay to a newspaper reflecting your views on censorship in libraries. Do you believe that certain materials, such as books, music, movies, magazines, etc., should be removed from the shelves if they are found offensive? Support your position with convincing arguments from your own experience, observations, and/or reading.</t>
+  </si>
+  <si>
+    <t>source dependent responses</t>
+  </si>
+  <si>
+    <t>Read "Rough Road Ahead" by Joe Kurmaski, from Metal Cowboy. Write a response that explains how the features of the setting affect the cyclist. In your response, include examples from the essay that support your conclusion.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 words response to the following prompt: Read "Rough Road Ahead" by Joe Kurmaski.  Write a response that explains how the features of the setting affect the cyclist.</t>
+  </si>
+  <si>
+    <t>Read Winter Hibiscus by Minfong Ho. Read the last paragraph of the story.
+"When they come back, Saeng vowed silently to herself, in the spring, when the snows melt and the geese return and this hibiscus is budding, then I will take that test again." 
+Write a response that explains why the author concludes the story with this paragraph. In your response, include details and examples from the story that support your ideas.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response to the following prompt: Read Winter Hibiscus by Minfong Ho. Read the last paragraph of the story.
+"When they come back, Saeng vowed silently to herself, in the spring, when the snows melt and the geese return and this hibiscus is budding, then I will take that test again." 
+Write a response that explains why the author concludes the story with this paragraph. In your response, include details and examples from the story that support your ideas.</t>
+  </si>
+  <si>
+    <t>Read Narciso Rodriguez from Home: The Blueprints of Our Lives. Describe the mood created by the author in the memoir. Support your answer with relevant and specific information from the memoir.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response to the following prompt: Read Narciso Rodriguez from Home: The Blueprints of Our Lives. Describe the mood created by the author in the memoir. Support your answer with relevant and specific information from the memoir.</t>
+  </si>
+  <si>
+    <t>Read The Mooring Mast by Marcia Amidon Lüsted. Based on the excerpt, describe the obstacles the builders of the Empire State Building faced in attempting to allow dirigibles to dock there. Support your answer with relevant and specific information from the excerpt.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response to the following prompt: Read The Mooring Mast by Marcia Amidon Lüsted. Based on the excerpt, describe the obstacles the builders of the Empire State Building faced in attempting to allow dirigibles to dock there. Support your answer with relevant and specific information from the excerpt.</t>
+  </si>
+  <si>
+    <t>Write about patience. Being patient means that you are understanding and tolerant. A patient person experience difficulties without complaining.
+Do only one of the following: write a story about a time when you were patient OR write a story about a time when someone you know was patient OR write a story in your own way about patience.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response to the following prompt: Write about patience. Being patient means that you are understanding and tolerant. A patient person experience difficulties without complaining.
+Do only one of the following: write a story about a time when you were patient OR write a story about a time when someone you know was patient OR write a story in your own way about patience.</t>
+  </si>
+  <si>
+    <t>We all understand the benefits of laughter. For example, someone once said, “Laughter is the shortest distance between two people.” Many other people believe that laughter is an important part of any relationship. Tell a true story in which laughter was one element or part.</t>
+  </si>
+  <si>
+    <t>Write a 200 to 500 word response to the following prompt: We all understand the benefits of laughter. For example, someone once said, “Laughter is the shortest distance between two people.” Many other people believe that laughter is an important part of any relationship. Tell a true story in which laughter was one element or part.</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/azure/cognitive-services/openai/concepts/prompt-engineering</t>
+  </si>
+  <si>
+    <r>
+      <t>Be Specific</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF161616"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Leave as little to interpretation as possible. Restrict the operational space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Be Descriptive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF161616"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Use analogies.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Double Down</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF161616"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Sometimes you may need to repeat yourself to the model. Give instructions before and after your primary content, use an instruction and a cue, etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Order Matters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF161616"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>. The order in which you present information to the model may impact the output. Whether you put instructions before your content (“summarize the following…”) or after (“summarize the above…”) can make a difference in output. Even the order of few-shot examples can matter. This is referred to as recency bias.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Give the model an “out”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF161616"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>. It can sometimes be helpful to give the model an alternative path if it is unable to complete the assigned task. For example, when asking a question over a piece of text you might include something like "respond with ‘not found’ if the answer is not present". This can help the model avoid generating false responses.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/main_classes/text_generation</t>
+  </si>
+  <si>
+    <t>API Company</t>
+  </si>
+  <si>
+    <t>Hugging Face</t>
+  </si>
+  <si>
+    <t>Deep AI</t>
+  </si>
+  <si>
+    <t>https://deepai.org/machine-learning-model/text-generator</t>
+  </si>
+  <si>
+    <t>https://textcortex.com/text-generation-api</t>
+  </si>
+  <si>
+    <t>Text Cortex</t>
+  </si>
+  <si>
+    <t>API General Link</t>
+  </si>
+  <si>
+    <t>Documentation Link</t>
+  </si>
+  <si>
+    <t>https://documenter.getpostman.com/view/936254/2s83tCLYi9#24be6895-850f-433b-80fd-312ac1acffad</t>
+  </si>
+  <si>
+    <t>Open AI</t>
+  </si>
+  <si>
+    <t>https://platform.openai.com/docs/guides/completion</t>
+  </si>
+  <si>
+    <t>NLP Cloud</t>
+  </si>
+  <si>
+    <t>https://nlpcloud.com/nlp-text-generation-api-gpt-neo-gpt-j-gpt-3-alternatives.html</t>
+  </si>
+  <si>
+    <t>https://platform.openai.com/docs/api-reference</t>
+  </si>
+  <si>
+    <t>Hugging Face Transformers Package</t>
+  </si>
+  <si>
+    <t>https://medium.com/the-side-hustle-club/generate-text-content-with-7-lines-of-python-and-ai-4031ef5da5bf</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/EleutherAI/gpt-j-6B</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/docs/transformers/v4.27.2/en/main_classes/text_generation#transformers.GenerationMixin.generate</t>
+  </si>
+  <si>
+    <t>Additional Link</t>
+  </si>
+  <si>
+    <t>https://platform.openai.com/docs/guides/completion/prompt-design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,6 +465,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF161616"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF161616"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -236,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,6 +523,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -567,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906EDF26-F271-FF4C-A21F-BA8AB3441038}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -779,4 +1064,794 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEFFF1E-E0B9-4148-91B1-E95D52153A6E}">
+  <dimension ref="A1:S16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="87.1640625" customWidth="1"/>
+    <col min="4" max="4" width="101.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="144" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="5">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1783</v>
+      </c>
+      <c r="G2" s="5">
+        <v>589</v>
+      </c>
+      <c r="H2" s="5">
+        <v>594</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5">
+        <v>1</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="144" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="5">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1800</v>
+      </c>
+      <c r="G3" s="5">
+        <v>600</v>
+      </c>
+      <c r="H3" s="5">
+        <v>600</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>6</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
+        <v>4</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>1</v>
+      </c>
+      <c r="R3" s="5">
+        <v>1</v>
+      </c>
+      <c r="S3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1726</v>
+      </c>
+      <c r="G4" s="5">
+        <v>568</v>
+      </c>
+      <c r="H4" s="5">
+        <v>564</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="128" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1772</v>
+      </c>
+      <c r="G5" s="5">
+        <v>586</v>
+      </c>
+      <c r="H5" s="5">
+        <v>590</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1805</v>
+      </c>
+      <c r="G6" s="5">
+        <v>601</v>
+      </c>
+      <c r="H6" s="5">
+        <v>600</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>4</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1800</v>
+      </c>
+      <c r="G7" s="5">
+        <v>600</v>
+      </c>
+      <c r="H7" s="5">
+        <v>600</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>4</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="5">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1569</v>
+      </c>
+      <c r="G8" s="5">
+        <v>441</v>
+      </c>
+      <c r="H8" s="5">
+        <v>454</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>30</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="5">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>723</v>
+      </c>
+      <c r="G9" s="5">
+        <v>233</v>
+      </c>
+      <c r="H9" s="5">
+        <v>252</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>60</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="P9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5">
+        <v>0</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="20" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD65A7-AE65-244A-BEB4-2AD1480CCC5C}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="62.1640625" customWidth="1"/>
+    <col min="3" max="3" width="85.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="D12" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="D13" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="D14" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="D15" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="D16" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
slight update to text generation script, dataset notes, and proposal.
</commit_message>
<xml_diff>
--- a/projectPlanning/datasetsNotes.xlsx
+++ b/projectPlanning/datasetsNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/projectPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE922010-6B76-B64B-B244-9AE4DAF3FFDB}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A579F2E7-8E3C-BE4B-A210-F87241E29978}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="133">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -434,10 +434,73 @@
     <t>https://huggingface.co/docs/transformers/v4.27.2/en/main_classes/text_generation#transformers.GenerationMixin.generate</t>
   </si>
   <si>
-    <t>Additional Link</t>
-  </si>
-  <si>
     <t>https://platform.openai.com/docs/guides/completion/prompt-design</t>
+  </si>
+  <si>
+    <t>https://ai.facebook.com/blog/large-language-model-llama-meta-ai/</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSfqNECQnMkycAp2jP4Z9TFX0cGR4uf7b_fBxjY_OjhJILlKGA/viewform</t>
+  </si>
+  <si>
+    <t>Meta's llama</t>
+  </si>
+  <si>
+    <t>NOT AVAILABLE RIGHT NOW</t>
+  </si>
+  <si>
+    <t>Cohere</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>AI21</t>
+  </si>
+  <si>
+    <t>BERT - is bad</t>
+  </si>
+  <si>
+    <t>NVIDIA nemo</t>
+  </si>
+  <si>
+    <t>Link Recommended by Piro</t>
+  </si>
+  <si>
+    <t>https://sourceforge.net/software/large-language-models/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Cloud - BARD </t>
+  </si>
+  <si>
+    <t>NOT AVAILABLE RIGHT NOW. WAITLIST</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/ai/generative-ai</t>
+  </si>
+  <si>
+    <t>essaysoft.net</t>
+  </si>
+  <si>
+    <t>longshot.ai</t>
+  </si>
+  <si>
+    <t>OpenAI</t>
+  </si>
+  <si>
+    <t>https://platform.openai.com/playground/p/8P6JA6XEx74NTvcRUngWKEYW?model=text-davinci-003</t>
+  </si>
+  <si>
+    <t>https://platform.openai.com/docs/api-reference/completions/create</t>
+  </si>
+  <si>
+    <t>API python link</t>
+  </si>
+  <si>
+    <t>https://github.com/openai/openai-python</t>
+  </si>
+  <si>
+    <t>Playground link</t>
   </si>
 </sst>
 </file>
@@ -480,10 +543,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF161616"/>
-      <name val="Helvetica Neue"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -513,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -531,6 +596,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1070,7 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEFFF1E-E0B9-4148-91B1-E95D52153A6E}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1731,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD65A7-AE65-244A-BEB4-2AD1480CCC5C}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1742,9 +1808,11 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="62.1640625" customWidth="1"/>
     <col min="3" max="3" width="85.1640625" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" customWidth="1"/>
+    <col min="5" max="5" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -1755,103 +1823,184 @@
         <v>99</v>
       </c>
       <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>106</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D11" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D12" s="8" t="s">
+    <row r="16" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="E16" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D13" s="8" t="s">
+    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D14" s="8" t="s">
+    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D15" s="8" t="s">
+    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D16" s="8" t="s">
+    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>90</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{33424B92-165A-3640-87FE-0CC08C6F199D}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{E9644E94-1C06-9A4C-8D68-7AF8BBD4B9C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add additional generated essays
</commit_message>
<xml_diff>
--- a/projectPlanning/datasetsNotes.xlsx
+++ b/projectPlanning/datasetsNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/projectPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A579F2E7-8E3C-BE4B-A210-F87241E29978}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B322A16-0F99-364C-BE93-19DC82661DF7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -613,10 +613,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1136,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEFFF1E-E0B9-4148-91B1-E95D52153A6E}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1799,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEAD65A7-AE65-244A-BEB4-2AD1480CCC5C}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
revise file structure, develop plots
</commit_message>
<xml_diff>
--- a/projectPlanning/datasetsNotes.xlsx
+++ b/projectPlanning/datasetsNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/projectPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1505993C-C060-F545-B357-D000C6EB3855}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A606A187-62D0-BA42-BAE9-9F798C3743E2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="132">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t xml:space="preserve">Yash's (TA) feedback on my question about our data: 1) focused on problem/concept first. 2) more data, better accuracy (features and sample size). 3) web scraping is an advanced thing so its more difficult. Is a good challenge and will look good, but is not compulsatory and is advanced/challenging. . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STARTING WITH THIS DATASET. </t>
   </si>
   <si>
     <t>essay_set</t>
@@ -584,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,6 +601,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,6 +620,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -919,21 +923,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906EDF26-F271-FF4C-A21F-BA8AB3441038}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -943,11 +947,11 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -957,14 +961,11 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -974,12 +975,12 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -989,12 +990,12 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1004,11 +1005,11 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1018,11 +1019,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="54" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="54" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1032,11 +1033,11 @@
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1057,79 +1058,79 @@
       <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13">
+      <c r="C11">
         <v>760</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C20" t="s">
         <v>25</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="26" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{FE61863E-14EA-3548-839B-01AFF8A88E98}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{FE61863E-14EA-3548-839B-01AFF8A88E98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1139,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEFFF1E-E0B9-4148-91B1-E95D52153A6E}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,61 +1152,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="144" x14ac:dyDescent="0.2">
@@ -1213,13 +1214,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="E2" s="5">
         <v>8</v>
@@ -1268,13 +1269,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -1327,13 +1328,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="E4" s="5">
         <v>10</v>
@@ -1382,13 +1383,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="E5" s="5">
         <v>10</v>
@@ -1437,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="5">
         <v>8</v>
@@ -1492,13 +1493,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="5">
         <v>10</v>
@@ -1547,13 +1548,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="E8" s="5">
         <v>7</v>
@@ -1602,13 +1603,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="E9" s="5">
         <v>10</v>
@@ -1817,186 +1818,186 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" t="s">
-        <v>97</v>
-      </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" t="s">
-        <v>126</v>
-      </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" t="s">
         <v>121</v>
-      </c>
-      <c r="C6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
         <v>106</v>
-      </c>
-      <c r="E7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
         <v>92</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
         <v>99</v>
       </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
         <v>101</v>
-      </c>
-      <c r="B11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>112</v>
-      </c>
       <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
         <v>109</v>
-      </c>
-      <c r="E12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
         <v>104</v>
-      </c>
-      <c r="B14" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="E16" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" t="s">
         <v>118</v>
-      </c>
-      <c r="B25" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>